<commit_message>
update the model scenarios spreadsheet
</commit_message>
<xml_diff>
--- a/data-raw/io model scenarios.xlsx
+++ b/data-raw/io model scenarios.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="32">
   <si>
     <t xml:space="preserve">year </t>
   </si>
@@ -46,9 +46,6 @@
   </si>
   <si>
     <t>tob.policy</t>
-  </si>
-  <si>
-    <t>NULL</t>
   </si>
   <si>
     <t>fte</t>
@@ -147,7 +144,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -169,6 +166,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="-0.24994659260841701"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59996337778862885"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -367,13 +370,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -426,6 +423,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -710,10 +713,10 @@
   <dimension ref="A1:CM573"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I27" sqref="I27"/>
+      <selection pane="bottomRight" activeCell="X42" sqref="X42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -723,8 +726,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:91" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="26" t="s">
-        <v>32</v>
+      <c r="A1" s="24" t="s">
+        <v>31</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>0</v>
@@ -744,56 +747,56 @@
       <c r="G1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="12" t="s">
-        <v>15</v>
+      <c r="H1" s="10" t="s">
+        <v>14</v>
       </c>
       <c r="I1" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="K1" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="L1" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="M1" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="N1" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="O1" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="P1" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q1" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="R1" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="S1" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="O1" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="P1" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q1" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="R1" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="S1" s="8" t="s">
+      <c r="T1" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="T1" s="8" t="s">
+      <c r="U1" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="U1" s="8" t="s">
+      <c r="V1" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="V1" s="8" t="s">
+      <c r="W1" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="W1" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="X1" s="10" t="s">
-        <v>16</v>
+      <c r="X1" s="9" t="s">
+        <v>15</v>
       </c>
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
@@ -864,7 +867,7 @@
       <c r="CM1" s="1"/>
     </row>
     <row r="2" spans="1:91" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="27">
+      <c r="A2" s="25">
         <v>1</v>
       </c>
       <c r="B2" s="3">
@@ -874,68 +877,52 @@
         <v>0</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
-      <c r="G2" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H2" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="I2" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="J2" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="K2" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="L2" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="M2" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="N2" s="23">
+      <c r="G2" s="4"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="13"/>
+      <c r="M2" s="13"/>
+      <c r="N2" s="21">
         <v>-0.1</v>
       </c>
-      <c r="O2" s="24">
+      <c r="O2" s="22">
         <v>-0.1</v>
       </c>
-      <c r="P2" s="24">
+      <c r="P2" s="22">
         <v>-0.1</v>
       </c>
-      <c r="Q2" s="24">
+      <c r="Q2" s="22">
         <v>-0.1</v>
       </c>
-      <c r="R2" s="24">
+      <c r="R2" s="22">
         <v>-0.1</v>
       </c>
-      <c r="S2" s="24">
+      <c r="S2" s="22">
         <v>-0.1</v>
       </c>
-      <c r="T2" s="24">
+      <c r="T2" s="22">
         <v>-0.1</v>
       </c>
-      <c r="U2" s="24">
+      <c r="U2" s="22">
         <v>-0.1</v>
       </c>
-      <c r="V2" s="24">
+      <c r="V2" s="22">
         <v>-0.1</v>
       </c>
-      <c r="W2" s="25">
+      <c r="W2" s="23">
         <v>-0.1</v>
       </c>
-      <c r="X2" s="9" t="s">
-        <v>7</v>
-      </c>
+      <c r="X2" s="27"/>
       <c r="Y2" s="1"/>
       <c r="Z2" s="1"/>
       <c r="AA2" s="1"/>
@@ -1005,7 +992,7 @@
       <c r="CM2" s="1"/>
     </row>
     <row r="3" spans="1:91" x14ac:dyDescent="0.25">
-      <c r="A3" s="27">
+      <c r="A3" s="25">
         <v>2</v>
       </c>
       <c r="B3" s="3">
@@ -1015,68 +1002,52 @@
         <v>0</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
-      <c r="G3" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H3" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="I3" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="J3" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="K3" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="L3" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="M3" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="N3" s="17">
+      <c r="G3" s="4"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="13"/>
+      <c r="K3" s="13"/>
+      <c r="L3" s="13"/>
+      <c r="M3" s="13"/>
+      <c r="N3" s="15">
         <v>-0.1</v>
       </c>
-      <c r="O3" s="18">
+      <c r="O3" s="16">
         <v>-0.1</v>
       </c>
-      <c r="P3" s="18">
+      <c r="P3" s="16">
         <v>-0.1</v>
       </c>
-      <c r="Q3" s="18">
+      <c r="Q3" s="16">
         <v>-0.1</v>
       </c>
-      <c r="R3" s="18">
+      <c r="R3" s="16">
         <v>-0.1</v>
       </c>
-      <c r="S3" s="18">
+      <c r="S3" s="16">
         <v>-0.1</v>
       </c>
-      <c r="T3" s="18">
+      <c r="T3" s="16">
         <v>-0.1</v>
       </c>
-      <c r="U3" s="18">
+      <c r="U3" s="16">
         <v>-0.1</v>
       </c>
-      <c r="V3" s="18">
+      <c r="V3" s="16">
         <v>-0.1</v>
       </c>
-      <c r="W3" s="19">
+      <c r="W3" s="17">
         <v>-0.1</v>
       </c>
-      <c r="X3" s="9" t="s">
-        <v>7</v>
-      </c>
+      <c r="X3" s="27"/>
       <c r="Y3" s="1"/>
       <c r="Z3" s="1"/>
       <c r="AA3" s="1"/>
@@ -1146,7 +1117,7 @@
       <c r="CM3" s="1"/>
     </row>
     <row r="4" spans="1:91" x14ac:dyDescent="0.25">
-      <c r="A4" s="27">
+      <c r="A4" s="25">
         <v>3</v>
       </c>
       <c r="B4" s="3">
@@ -1156,68 +1127,52 @@
         <v>0</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
-      <c r="G4" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H4" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="I4" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="J4" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="K4" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="L4" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="M4" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="N4" s="17">
+      <c r="G4" s="4"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="13"/>
+      <c r="K4" s="13"/>
+      <c r="L4" s="13"/>
+      <c r="M4" s="13"/>
+      <c r="N4" s="15">
         <v>-0.1</v>
       </c>
-      <c r="O4" s="18">
+      <c r="O4" s="16">
         <v>-0.1</v>
       </c>
-      <c r="P4" s="18">
+      <c r="P4" s="16">
         <v>-0.1</v>
       </c>
-      <c r="Q4" s="18">
+      <c r="Q4" s="16">
         <v>-0.1</v>
       </c>
-      <c r="R4" s="18">
+      <c r="R4" s="16">
         <v>-0.1</v>
       </c>
-      <c r="S4" s="18">
+      <c r="S4" s="16">
         <v>-0.1</v>
       </c>
-      <c r="T4" s="18">
+      <c r="T4" s="16">
         <v>-0.1</v>
       </c>
-      <c r="U4" s="18">
+      <c r="U4" s="16">
         <v>-0.1</v>
       </c>
-      <c r="V4" s="18">
+      <c r="V4" s="16">
         <v>-0.1</v>
       </c>
-      <c r="W4" s="19">
+      <c r="W4" s="17">
         <v>-0.1</v>
       </c>
-      <c r="X4" s="9" t="s">
-        <v>7</v>
-      </c>
+      <c r="X4" s="27"/>
       <c r="Y4" s="1"/>
       <c r="Z4" s="1"/>
       <c r="AA4" s="1"/>
@@ -1287,7 +1242,7 @@
       <c r="CM4" s="1"/>
     </row>
     <row r="5" spans="1:91" x14ac:dyDescent="0.25">
-      <c r="A5" s="27">
+      <c r="A5" s="25">
         <v>4</v>
       </c>
       <c r="B5" s="3">
@@ -1297,68 +1252,52 @@
         <v>0</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
-      <c r="G5" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H5" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="I5" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="J5" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="K5" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="L5" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="M5" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="N5" s="17">
+      <c r="G5" s="4"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="13"/>
+      <c r="L5" s="13"/>
+      <c r="M5" s="13"/>
+      <c r="N5" s="15">
         <v>-0.1</v>
       </c>
-      <c r="O5" s="18">
+      <c r="O5" s="16">
         <v>-0.1</v>
       </c>
-      <c r="P5" s="18">
+      <c r="P5" s="16">
         <v>-0.1</v>
       </c>
-      <c r="Q5" s="18">
+      <c r="Q5" s="16">
         <v>-0.1</v>
       </c>
-      <c r="R5" s="18">
+      <c r="R5" s="16">
         <v>-0.1</v>
       </c>
-      <c r="S5" s="18">
+      <c r="S5" s="16">
         <v>-0.1</v>
       </c>
-      <c r="T5" s="18">
+      <c r="T5" s="16">
         <v>-0.1</v>
       </c>
-      <c r="U5" s="18">
+      <c r="U5" s="16">
         <v>-0.1</v>
       </c>
-      <c r="V5" s="18">
+      <c r="V5" s="16">
         <v>-0.1</v>
       </c>
-      <c r="W5" s="19">
+      <c r="W5" s="17">
         <v>-0.1</v>
       </c>
-      <c r="X5" s="9" t="s">
-        <v>7</v>
-      </c>
+      <c r="X5" s="27"/>
       <c r="Y5" s="1"/>
       <c r="Z5" s="1"/>
       <c r="AA5" s="1"/>
@@ -1428,7 +1367,7 @@
       <c r="CM5" s="1"/>
     </row>
     <row r="6" spans="1:91" x14ac:dyDescent="0.25">
-      <c r="A6" s="27">
+      <c r="A6" s="25">
         <v>5</v>
       </c>
       <c r="B6" s="3">
@@ -1438,68 +1377,52 @@
         <v>0</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
-      <c r="G6" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H6" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="I6" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="J6" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="K6" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="L6" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="M6" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="N6" s="17">
+      <c r="G6" s="4"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="13"/>
+      <c r="L6" s="13"/>
+      <c r="M6" s="13"/>
+      <c r="N6" s="15">
         <v>-0.1</v>
       </c>
-      <c r="O6" s="18">
+      <c r="O6" s="16">
         <v>-0.1</v>
       </c>
-      <c r="P6" s="18">
+      <c r="P6" s="16">
         <v>-0.1</v>
       </c>
-      <c r="Q6" s="18">
+      <c r="Q6" s="16">
         <v>-0.1</v>
       </c>
-      <c r="R6" s="18">
+      <c r="R6" s="16">
         <v>-0.1</v>
       </c>
-      <c r="S6" s="18">
+      <c r="S6" s="16">
         <v>-0.1</v>
       </c>
-      <c r="T6" s="18">
+      <c r="T6" s="16">
         <v>-0.1</v>
       </c>
-      <c r="U6" s="18">
+      <c r="U6" s="16">
         <v>-0.1</v>
       </c>
-      <c r="V6" s="18">
+      <c r="V6" s="16">
         <v>-0.1</v>
       </c>
-      <c r="W6" s="19">
+      <c r="W6" s="17">
         <v>-0.1</v>
       </c>
-      <c r="X6" s="9" t="s">
-        <v>7</v>
-      </c>
+      <c r="X6" s="27"/>
       <c r="Y6" s="1"/>
       <c r="Z6" s="1"/>
       <c r="AA6" s="1"/>
@@ -1569,7 +1492,7 @@
       <c r="CM6" s="1"/>
     </row>
     <row r="7" spans="1:91" x14ac:dyDescent="0.25">
-      <c r="A7" s="27">
+      <c r="A7" s="25">
         <v>6</v>
       </c>
       <c r="B7" s="3">
@@ -1579,68 +1502,52 @@
         <v>0</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
-      <c r="G7" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H7" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="I7" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="J7" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="K7" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="L7" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="M7" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="N7" s="17">
+      <c r="G7" s="4"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="13"/>
+      <c r="K7" s="13"/>
+      <c r="L7" s="13"/>
+      <c r="M7" s="13"/>
+      <c r="N7" s="15">
         <v>-0.1</v>
       </c>
-      <c r="O7" s="18">
+      <c r="O7" s="16">
         <v>-0.1</v>
       </c>
-      <c r="P7" s="18">
+      <c r="P7" s="16">
         <v>-0.1</v>
       </c>
-      <c r="Q7" s="18">
+      <c r="Q7" s="16">
         <v>-0.1</v>
       </c>
-      <c r="R7" s="18">
+      <c r="R7" s="16">
         <v>-0.1</v>
       </c>
-      <c r="S7" s="18">
+      <c r="S7" s="16">
         <v>-0.1</v>
       </c>
-      <c r="T7" s="18">
+      <c r="T7" s="16">
         <v>-0.1</v>
       </c>
-      <c r="U7" s="18">
+      <c r="U7" s="16">
         <v>-0.1</v>
       </c>
-      <c r="V7" s="18">
+      <c r="V7" s="16">
         <v>-0.1</v>
       </c>
-      <c r="W7" s="19">
+      <c r="W7" s="17">
         <v>-0.1</v>
       </c>
-      <c r="X7" s="9" t="s">
-        <v>7</v>
-      </c>
+      <c r="X7" s="27"/>
       <c r="Y7" s="1"/>
       <c r="Z7" s="1"/>
       <c r="AA7" s="1"/>
@@ -1710,7 +1617,7 @@
       <c r="CM7" s="1"/>
     </row>
     <row r="8" spans="1:91" x14ac:dyDescent="0.25">
-      <c r="A8" s="27">
+      <c r="A8" s="25">
         <v>7</v>
       </c>
       <c r="B8" s="3">
@@ -1720,68 +1627,52 @@
         <v>0</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
-      <c r="G8" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H8" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="I8" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="J8" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="K8" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="L8" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="M8" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="N8" s="17">
+      <c r="G8" s="4"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="13"/>
+      <c r="K8" s="13"/>
+      <c r="L8" s="13"/>
+      <c r="M8" s="13"/>
+      <c r="N8" s="15">
         <v>-0.1</v>
       </c>
-      <c r="O8" s="18">
+      <c r="O8" s="16">
         <v>-0.1</v>
       </c>
-      <c r="P8" s="18">
+      <c r="P8" s="16">
         <v>-0.1</v>
       </c>
-      <c r="Q8" s="18">
+      <c r="Q8" s="16">
         <v>-0.1</v>
       </c>
-      <c r="R8" s="18">
+      <c r="R8" s="16">
         <v>-0.1</v>
       </c>
-      <c r="S8" s="18">
+      <c r="S8" s="16">
         <v>-0.1</v>
       </c>
-      <c r="T8" s="18">
+      <c r="T8" s="16">
         <v>-0.1</v>
       </c>
-      <c r="U8" s="18">
+      <c r="U8" s="16">
         <v>-0.1</v>
       </c>
-      <c r="V8" s="18">
+      <c r="V8" s="16">
         <v>-0.1</v>
       </c>
-      <c r="W8" s="19">
+      <c r="W8" s="17">
         <v>-0.1</v>
       </c>
-      <c r="X8" s="9" t="s">
-        <v>7</v>
-      </c>
+      <c r="X8" s="27"/>
       <c r="Y8" s="1"/>
       <c r="Z8" s="1"/>
       <c r="AA8" s="1"/>
@@ -1851,7 +1742,7 @@
       <c r="CM8" s="1"/>
     </row>
     <row r="9" spans="1:91" x14ac:dyDescent="0.25">
-      <c r="A9" s="27">
+      <c r="A9" s="25">
         <v>8</v>
       </c>
       <c r="B9" s="3">
@@ -1861,68 +1752,52 @@
         <v>0</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
-      <c r="G9" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H9" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="I9" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="J9" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="K9" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="L9" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="M9" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="N9" s="17">
+      <c r="G9" s="4"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="13"/>
+      <c r="K9" s="13"/>
+      <c r="L9" s="13"/>
+      <c r="M9" s="13"/>
+      <c r="N9" s="15">
         <v>-0.1</v>
       </c>
-      <c r="O9" s="18">
+      <c r="O9" s="16">
         <v>-0.1</v>
       </c>
-      <c r="P9" s="18">
+      <c r="P9" s="16">
         <v>-0.1</v>
       </c>
-      <c r="Q9" s="18">
+      <c r="Q9" s="16">
         <v>-0.1</v>
       </c>
-      <c r="R9" s="18">
+      <c r="R9" s="16">
         <v>-0.1</v>
       </c>
-      <c r="S9" s="18">
+      <c r="S9" s="16">
         <v>-0.1</v>
       </c>
-      <c r="T9" s="18">
+      <c r="T9" s="16">
         <v>-0.1</v>
       </c>
-      <c r="U9" s="18">
+      <c r="U9" s="16">
         <v>-0.1</v>
       </c>
-      <c r="V9" s="18">
+      <c r="V9" s="16">
         <v>-0.1</v>
       </c>
-      <c r="W9" s="19">
+      <c r="W9" s="17">
         <v>-0.1</v>
       </c>
-      <c r="X9" s="9" t="s">
-        <v>7</v>
-      </c>
+      <c r="X9" s="27"/>
       <c r="Y9" s="1"/>
       <c r="Z9" s="1"/>
       <c r="AA9" s="1"/>
@@ -1992,7 +1867,7 @@
       <c r="CM9" s="1"/>
     </row>
     <row r="10" spans="1:91" x14ac:dyDescent="0.25">
-      <c r="A10" s="27">
+      <c r="A10" s="25">
         <v>9</v>
       </c>
       <c r="B10" s="3">
@@ -2002,68 +1877,52 @@
         <v>0</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
-      <c r="G10" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H10" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="I10" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="J10" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="K10" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="L10" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="M10" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="N10" s="17">
+      <c r="G10" s="4"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="13"/>
+      <c r="K10" s="13"/>
+      <c r="L10" s="13"/>
+      <c r="M10" s="13"/>
+      <c r="N10" s="15">
         <v>-0.1</v>
       </c>
-      <c r="O10" s="18">
+      <c r="O10" s="16">
         <v>-0.1</v>
       </c>
-      <c r="P10" s="18">
+      <c r="P10" s="16">
         <v>-0.1</v>
       </c>
-      <c r="Q10" s="18">
+      <c r="Q10" s="16">
         <v>-0.1</v>
       </c>
-      <c r="R10" s="18">
+      <c r="R10" s="16">
         <v>-0.1</v>
       </c>
-      <c r="S10" s="18">
+      <c r="S10" s="16">
         <v>-0.1</v>
       </c>
-      <c r="T10" s="18">
+      <c r="T10" s="16">
         <v>-0.1</v>
       </c>
-      <c r="U10" s="18">
+      <c r="U10" s="16">
         <v>-0.1</v>
       </c>
-      <c r="V10" s="18">
+      <c r="V10" s="16">
         <v>-0.1</v>
       </c>
-      <c r="W10" s="19">
+      <c r="W10" s="17">
         <v>-0.1</v>
       </c>
-      <c r="X10" s="9" t="s">
-        <v>7</v>
-      </c>
+      <c r="X10" s="27"/>
       <c r="Y10" s="1"/>
       <c r="Z10" s="1"/>
       <c r="AA10" s="1"/>
@@ -2133,7 +1992,7 @@
       <c r="CM10" s="1"/>
     </row>
     <row r="11" spans="1:91" x14ac:dyDescent="0.25">
-      <c r="A11" s="27">
+      <c r="A11" s="25">
         <v>10</v>
       </c>
       <c r="B11" s="3">
@@ -2143,68 +2002,52 @@
         <v>0</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
-      <c r="G11" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H11" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="I11" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="J11" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="K11" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="L11" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="M11" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="N11" s="17">
+      <c r="G11" s="4"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="13"/>
+      <c r="K11" s="13"/>
+      <c r="L11" s="13"/>
+      <c r="M11" s="13"/>
+      <c r="N11" s="15">
         <v>-0.1</v>
       </c>
-      <c r="O11" s="18">
+      <c r="O11" s="16">
         <v>-0.1</v>
       </c>
-      <c r="P11" s="18">
+      <c r="P11" s="16">
         <v>-0.1</v>
       </c>
-      <c r="Q11" s="18">
+      <c r="Q11" s="16">
         <v>-0.1</v>
       </c>
-      <c r="R11" s="18">
+      <c r="R11" s="16">
         <v>-0.1</v>
       </c>
-      <c r="S11" s="18">
+      <c r="S11" s="16">
         <v>-0.1</v>
       </c>
-      <c r="T11" s="18">
+      <c r="T11" s="16">
         <v>-0.1</v>
       </c>
-      <c r="U11" s="18">
+      <c r="U11" s="16">
         <v>-0.1</v>
       </c>
-      <c r="V11" s="18">
+      <c r="V11" s="16">
         <v>-0.1</v>
       </c>
-      <c r="W11" s="19">
+      <c r="W11" s="17">
         <v>-0.1</v>
       </c>
-      <c r="X11" s="9" t="s">
-        <v>7</v>
-      </c>
+      <c r="X11" s="27"/>
       <c r="Y11" s="1"/>
       <c r="Z11" s="1"/>
       <c r="AA11" s="1"/>
@@ -2274,7 +2117,7 @@
       <c r="CM11" s="1"/>
     </row>
     <row r="12" spans="1:91" x14ac:dyDescent="0.25">
-      <c r="A12" s="27">
+      <c r="A12" s="25">
         <v>11</v>
       </c>
       <c r="B12" s="3"/>
@@ -2283,23 +2126,23 @@
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
-      <c r="H12" s="13"/>
-      <c r="I12" s="15"/>
-      <c r="J12" s="15"/>
-      <c r="K12" s="15"/>
-      <c r="L12" s="15"/>
-      <c r="M12" s="15"/>
-      <c r="N12" s="17"/>
-      <c r="O12" s="18"/>
-      <c r="P12" s="18"/>
-      <c r="Q12" s="18"/>
-      <c r="R12" s="18"/>
-      <c r="S12" s="18"/>
-      <c r="T12" s="18"/>
-      <c r="U12" s="18"/>
-      <c r="V12" s="18"/>
-      <c r="W12" s="19"/>
-      <c r="X12" s="9"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="13"/>
+      <c r="J12" s="13"/>
+      <c r="K12" s="13"/>
+      <c r="L12" s="13"/>
+      <c r="M12" s="13"/>
+      <c r="N12" s="15"/>
+      <c r="O12" s="16"/>
+      <c r="P12" s="16"/>
+      <c r="Q12" s="16"/>
+      <c r="R12" s="16"/>
+      <c r="S12" s="16"/>
+      <c r="T12" s="16"/>
+      <c r="U12" s="16"/>
+      <c r="V12" s="16"/>
+      <c r="W12" s="17"/>
+      <c r="X12" s="27"/>
       <c r="Y12" s="1"/>
       <c r="Z12" s="1"/>
       <c r="AA12" s="1"/>
@@ -2369,7 +2212,7 @@
       <c r="CM12" s="1"/>
     </row>
     <row r="13" spans="1:91" x14ac:dyDescent="0.25">
-      <c r="A13" s="27">
+      <c r="A13" s="25">
         <v>12</v>
       </c>
       <c r="B13" s="3"/>
@@ -2378,23 +2221,23 @@
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
-      <c r="H13" s="13"/>
-      <c r="I13" s="15"/>
-      <c r="J13" s="15"/>
-      <c r="K13" s="15"/>
-      <c r="L13" s="15"/>
-      <c r="M13" s="15"/>
-      <c r="N13" s="17"/>
-      <c r="O13" s="18"/>
-      <c r="P13" s="18"/>
-      <c r="Q13" s="18"/>
-      <c r="R13" s="18"/>
-      <c r="S13" s="18"/>
-      <c r="T13" s="18"/>
-      <c r="U13" s="18"/>
-      <c r="V13" s="18"/>
-      <c r="W13" s="19"/>
-      <c r="X13" s="9"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="13"/>
+      <c r="J13" s="13"/>
+      <c r="K13" s="13"/>
+      <c r="L13" s="13"/>
+      <c r="M13" s="13"/>
+      <c r="N13" s="15"/>
+      <c r="O13" s="16"/>
+      <c r="P13" s="16"/>
+      <c r="Q13" s="16"/>
+      <c r="R13" s="16"/>
+      <c r="S13" s="16"/>
+      <c r="T13" s="16"/>
+      <c r="U13" s="16"/>
+      <c r="V13" s="16"/>
+      <c r="W13" s="17"/>
+      <c r="X13" s="27"/>
       <c r="Y13" s="1"/>
       <c r="Z13" s="1"/>
       <c r="AA13" s="1"/>
@@ -2464,7 +2307,7 @@
       <c r="CM13" s="1"/>
     </row>
     <row r="14" spans="1:91" x14ac:dyDescent="0.25">
-      <c r="A14" s="27">
+      <c r="A14" s="25">
         <v>13</v>
       </c>
       <c r="B14" s="3"/>
@@ -2473,23 +2316,23 @@
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
-      <c r="H14" s="13"/>
-      <c r="I14" s="15"/>
-      <c r="J14" s="15"/>
-      <c r="K14" s="15"/>
-      <c r="L14" s="15"/>
-      <c r="M14" s="15"/>
-      <c r="N14" s="17"/>
-      <c r="O14" s="18"/>
-      <c r="P14" s="18"/>
-      <c r="Q14" s="18"/>
-      <c r="R14" s="18"/>
-      <c r="S14" s="18"/>
-      <c r="T14" s="18"/>
-      <c r="U14" s="18"/>
-      <c r="V14" s="18"/>
-      <c r="W14" s="19"/>
-      <c r="X14" s="9"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="13"/>
+      <c r="J14" s="13"/>
+      <c r="K14" s="13"/>
+      <c r="L14" s="13"/>
+      <c r="M14" s="13"/>
+      <c r="N14" s="15"/>
+      <c r="O14" s="16"/>
+      <c r="P14" s="16"/>
+      <c r="Q14" s="16"/>
+      <c r="R14" s="16"/>
+      <c r="S14" s="16"/>
+      <c r="T14" s="16"/>
+      <c r="U14" s="16"/>
+      <c r="V14" s="16"/>
+      <c r="W14" s="17"/>
+      <c r="X14" s="27"/>
       <c r="Y14" s="1"/>
       <c r="Z14" s="1"/>
       <c r="AA14" s="1"/>
@@ -2559,7 +2402,7 @@
       <c r="CM14" s="1"/>
     </row>
     <row r="15" spans="1:91" x14ac:dyDescent="0.25">
-      <c r="A15" s="27">
+      <c r="A15" s="25">
         <v>14</v>
       </c>
       <c r="B15" s="3"/>
@@ -2568,23 +2411,23 @@
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
-      <c r="H15" s="13"/>
-      <c r="I15" s="15"/>
-      <c r="J15" s="15"/>
-      <c r="K15" s="15"/>
-      <c r="L15" s="15"/>
-      <c r="M15" s="15"/>
-      <c r="N15" s="17"/>
-      <c r="O15" s="18"/>
-      <c r="P15" s="18"/>
-      <c r="Q15" s="18"/>
-      <c r="R15" s="18"/>
-      <c r="S15" s="18"/>
-      <c r="T15" s="18"/>
-      <c r="U15" s="18"/>
-      <c r="V15" s="18"/>
-      <c r="W15" s="19"/>
-      <c r="X15" s="9"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="13"/>
+      <c r="K15" s="13"/>
+      <c r="L15" s="13"/>
+      <c r="M15" s="13"/>
+      <c r="N15" s="15"/>
+      <c r="O15" s="16"/>
+      <c r="P15" s="16"/>
+      <c r="Q15" s="16"/>
+      <c r="R15" s="16"/>
+      <c r="S15" s="16"/>
+      <c r="T15" s="16"/>
+      <c r="U15" s="16"/>
+      <c r="V15" s="16"/>
+      <c r="W15" s="17"/>
+      <c r="X15" s="27"/>
       <c r="Y15" s="1"/>
       <c r="Z15" s="1"/>
       <c r="AA15" s="1"/>
@@ -2654,7 +2497,7 @@
       <c r="CM15" s="1"/>
     </row>
     <row r="16" spans="1:91" x14ac:dyDescent="0.25">
-      <c r="A16" s="27">
+      <c r="A16" s="25">
         <v>15</v>
       </c>
       <c r="B16" s="3"/>
@@ -2663,23 +2506,23 @@
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
-      <c r="H16" s="13"/>
-      <c r="I16" s="15"/>
-      <c r="J16" s="15"/>
-      <c r="K16" s="15"/>
-      <c r="L16" s="15"/>
-      <c r="M16" s="15"/>
-      <c r="N16" s="17"/>
-      <c r="O16" s="18"/>
-      <c r="P16" s="18"/>
-      <c r="Q16" s="18"/>
-      <c r="R16" s="18"/>
-      <c r="S16" s="18"/>
-      <c r="T16" s="18"/>
-      <c r="U16" s="18"/>
-      <c r="V16" s="18"/>
-      <c r="W16" s="19"/>
-      <c r="X16" s="9"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="13"/>
+      <c r="J16" s="13"/>
+      <c r="K16" s="13"/>
+      <c r="L16" s="13"/>
+      <c r="M16" s="13"/>
+      <c r="N16" s="15"/>
+      <c r="O16" s="16"/>
+      <c r="P16" s="16"/>
+      <c r="Q16" s="16"/>
+      <c r="R16" s="16"/>
+      <c r="S16" s="16"/>
+      <c r="T16" s="16"/>
+      <c r="U16" s="16"/>
+      <c r="V16" s="16"/>
+      <c r="W16" s="17"/>
+      <c r="X16" s="27"/>
       <c r="Y16" s="1"/>
       <c r="Z16" s="1"/>
       <c r="AA16" s="1"/>
@@ -2749,7 +2592,7 @@
       <c r="CM16" s="1"/>
     </row>
     <row r="17" spans="1:91" x14ac:dyDescent="0.25">
-      <c r="A17" s="27">
+      <c r="A17" s="25">
         <v>16</v>
       </c>
       <c r="B17" s="3"/>
@@ -2758,23 +2601,23 @@
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
-      <c r="H17" s="13"/>
-      <c r="I17" s="15"/>
-      <c r="J17" s="15"/>
-      <c r="K17" s="15"/>
-      <c r="L17" s="15"/>
-      <c r="M17" s="15"/>
-      <c r="N17" s="17"/>
-      <c r="O17" s="18"/>
-      <c r="P17" s="18"/>
-      <c r="Q17" s="18"/>
-      <c r="R17" s="18"/>
-      <c r="S17" s="18"/>
-      <c r="T17" s="18"/>
-      <c r="U17" s="18"/>
-      <c r="V17" s="18"/>
-      <c r="W17" s="19"/>
-      <c r="X17" s="9"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="13"/>
+      <c r="J17" s="13"/>
+      <c r="K17" s="13"/>
+      <c r="L17" s="13"/>
+      <c r="M17" s="13"/>
+      <c r="N17" s="15"/>
+      <c r="O17" s="16"/>
+      <c r="P17" s="16"/>
+      <c r="Q17" s="16"/>
+      <c r="R17" s="16"/>
+      <c r="S17" s="16"/>
+      <c r="T17" s="16"/>
+      <c r="U17" s="16"/>
+      <c r="V17" s="16"/>
+      <c r="W17" s="17"/>
+      <c r="X17" s="27"/>
       <c r="Y17" s="1"/>
       <c r="Z17" s="1"/>
       <c r="AA17" s="1"/>
@@ -2844,7 +2687,7 @@
       <c r="CM17" s="1"/>
     </row>
     <row r="18" spans="1:91" x14ac:dyDescent="0.25">
-      <c r="A18" s="27">
+      <c r="A18" s="25">
         <v>17</v>
       </c>
       <c r="B18" s="3"/>
@@ -2853,23 +2696,23 @@
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
       <c r="G18" s="4"/>
-      <c r="H18" s="13"/>
-      <c r="I18" s="15"/>
-      <c r="J18" s="15"/>
-      <c r="K18" s="15"/>
-      <c r="L18" s="15"/>
-      <c r="M18" s="15"/>
-      <c r="N18" s="17"/>
-      <c r="O18" s="18"/>
-      <c r="P18" s="18"/>
-      <c r="Q18" s="18"/>
-      <c r="R18" s="18"/>
-      <c r="S18" s="18"/>
-      <c r="T18" s="18"/>
-      <c r="U18" s="18"/>
-      <c r="V18" s="18"/>
-      <c r="W18" s="19"/>
-      <c r="X18" s="9"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="13"/>
+      <c r="J18" s="13"/>
+      <c r="K18" s="13"/>
+      <c r="L18" s="13"/>
+      <c r="M18" s="13"/>
+      <c r="N18" s="15"/>
+      <c r="O18" s="16"/>
+      <c r="P18" s="16"/>
+      <c r="Q18" s="16"/>
+      <c r="R18" s="16"/>
+      <c r="S18" s="16"/>
+      <c r="T18" s="16"/>
+      <c r="U18" s="16"/>
+      <c r="V18" s="16"/>
+      <c r="W18" s="17"/>
+      <c r="X18" s="27"/>
       <c r="Y18" s="1"/>
       <c r="Z18" s="1"/>
       <c r="AA18" s="1"/>
@@ -2939,7 +2782,7 @@
       <c r="CM18" s="1"/>
     </row>
     <row r="19" spans="1:91" x14ac:dyDescent="0.25">
-      <c r="A19" s="27">
+      <c r="A19" s="25">
         <v>18</v>
       </c>
       <c r="B19" s="3"/>
@@ -2948,23 +2791,23 @@
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
-      <c r="H19" s="13"/>
-      <c r="I19" s="15"/>
-      <c r="J19" s="15"/>
-      <c r="K19" s="15"/>
-      <c r="L19" s="15"/>
-      <c r="M19" s="15"/>
-      <c r="N19" s="17"/>
-      <c r="O19" s="18"/>
-      <c r="P19" s="18"/>
-      <c r="Q19" s="18"/>
-      <c r="R19" s="18"/>
-      <c r="S19" s="18"/>
-      <c r="T19" s="18"/>
-      <c r="U19" s="18"/>
-      <c r="V19" s="18"/>
-      <c r="W19" s="19"/>
-      <c r="X19" s="9"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="13"/>
+      <c r="J19" s="13"/>
+      <c r="K19" s="13"/>
+      <c r="L19" s="13"/>
+      <c r="M19" s="13"/>
+      <c r="N19" s="15"/>
+      <c r="O19" s="16"/>
+      <c r="P19" s="16"/>
+      <c r="Q19" s="16"/>
+      <c r="R19" s="16"/>
+      <c r="S19" s="16"/>
+      <c r="T19" s="16"/>
+      <c r="U19" s="16"/>
+      <c r="V19" s="16"/>
+      <c r="W19" s="17"/>
+      <c r="X19" s="27"/>
       <c r="Y19" s="1"/>
       <c r="Z19" s="1"/>
       <c r="AA19" s="1"/>
@@ -3034,7 +2877,7 @@
       <c r="CM19" s="1"/>
     </row>
     <row r="20" spans="1:91" x14ac:dyDescent="0.25">
-      <c r="A20" s="27">
+      <c r="A20" s="25">
         <v>19</v>
       </c>
       <c r="B20" s="3"/>
@@ -3043,23 +2886,23 @@
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
-      <c r="H20" s="13"/>
-      <c r="I20" s="15"/>
-      <c r="J20" s="15"/>
-      <c r="K20" s="15"/>
-      <c r="L20" s="15"/>
-      <c r="M20" s="15"/>
-      <c r="N20" s="17"/>
-      <c r="O20" s="18"/>
-      <c r="P20" s="18"/>
-      <c r="Q20" s="18"/>
-      <c r="R20" s="18"/>
-      <c r="S20" s="18"/>
-      <c r="T20" s="18"/>
-      <c r="U20" s="18"/>
-      <c r="V20" s="18"/>
-      <c r="W20" s="19"/>
-      <c r="X20" s="9"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="13"/>
+      <c r="J20" s="13"/>
+      <c r="K20" s="13"/>
+      <c r="L20" s="13"/>
+      <c r="M20" s="13"/>
+      <c r="N20" s="15"/>
+      <c r="O20" s="16"/>
+      <c r="P20" s="16"/>
+      <c r="Q20" s="16"/>
+      <c r="R20" s="16"/>
+      <c r="S20" s="16"/>
+      <c r="T20" s="16"/>
+      <c r="U20" s="16"/>
+      <c r="V20" s="16"/>
+      <c r="W20" s="17"/>
+      <c r="X20" s="27"/>
       <c r="Y20" s="1"/>
       <c r="Z20" s="1"/>
       <c r="AA20" s="1"/>
@@ -3129,7 +2972,7 @@
       <c r="CM20" s="1"/>
     </row>
     <row r="21" spans="1:91" x14ac:dyDescent="0.25">
-      <c r="A21" s="27">
+      <c r="A21" s="25">
         <v>20</v>
       </c>
       <c r="B21" s="3"/>
@@ -3138,23 +2981,23 @@
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
-      <c r="H21" s="13"/>
-      <c r="I21" s="15"/>
-      <c r="J21" s="15"/>
-      <c r="K21" s="15"/>
-      <c r="L21" s="15"/>
-      <c r="M21" s="15"/>
-      <c r="N21" s="17"/>
-      <c r="O21" s="18"/>
-      <c r="P21" s="18"/>
-      <c r="Q21" s="18"/>
-      <c r="R21" s="18"/>
-      <c r="S21" s="18"/>
-      <c r="T21" s="18"/>
-      <c r="U21" s="18"/>
-      <c r="V21" s="18"/>
-      <c r="W21" s="19"/>
-      <c r="X21" s="9"/>
+      <c r="H21" s="11"/>
+      <c r="I21" s="13"/>
+      <c r="J21" s="13"/>
+      <c r="K21" s="13"/>
+      <c r="L21" s="13"/>
+      <c r="M21" s="13"/>
+      <c r="N21" s="15"/>
+      <c r="O21" s="16"/>
+      <c r="P21" s="16"/>
+      <c r="Q21" s="16"/>
+      <c r="R21" s="16"/>
+      <c r="S21" s="16"/>
+      <c r="T21" s="16"/>
+      <c r="U21" s="16"/>
+      <c r="V21" s="16"/>
+      <c r="W21" s="17"/>
+      <c r="X21" s="27"/>
       <c r="Y21" s="1"/>
       <c r="Z21" s="1"/>
       <c r="AA21" s="1"/>
@@ -3224,7 +3067,7 @@
       <c r="CM21" s="1"/>
     </row>
     <row r="22" spans="1:91" x14ac:dyDescent="0.25">
-      <c r="A22" s="27">
+      <c r="A22" s="25">
         <v>21</v>
       </c>
       <c r="B22" s="3"/>
@@ -3233,23 +3076,23 @@
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
-      <c r="H22" s="13"/>
-      <c r="I22" s="15"/>
-      <c r="J22" s="15"/>
-      <c r="K22" s="15"/>
-      <c r="L22" s="15"/>
-      <c r="M22" s="15"/>
-      <c r="N22" s="17"/>
-      <c r="O22" s="18"/>
-      <c r="P22" s="18"/>
-      <c r="Q22" s="18"/>
-      <c r="R22" s="18"/>
-      <c r="S22" s="18"/>
-      <c r="T22" s="18"/>
-      <c r="U22" s="18"/>
-      <c r="V22" s="18"/>
-      <c r="W22" s="19"/>
-      <c r="X22" s="9"/>
+      <c r="H22" s="11"/>
+      <c r="I22" s="13"/>
+      <c r="J22" s="13"/>
+      <c r="K22" s="13"/>
+      <c r="L22" s="13"/>
+      <c r="M22" s="13"/>
+      <c r="N22" s="15"/>
+      <c r="O22" s="16"/>
+      <c r="P22" s="16"/>
+      <c r="Q22" s="16"/>
+      <c r="R22" s="16"/>
+      <c r="S22" s="16"/>
+      <c r="T22" s="16"/>
+      <c r="U22" s="16"/>
+      <c r="V22" s="16"/>
+      <c r="W22" s="17"/>
+      <c r="X22" s="27"/>
       <c r="Y22" s="1"/>
       <c r="Z22" s="1"/>
       <c r="AA22" s="1"/>
@@ -3319,7 +3162,7 @@
       <c r="CM22" s="1"/>
     </row>
     <row r="23" spans="1:91" x14ac:dyDescent="0.25">
-      <c r="A23" s="27">
+      <c r="A23" s="25">
         <v>22</v>
       </c>
       <c r="B23" s="3"/>
@@ -3328,23 +3171,23 @@
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
-      <c r="H23" s="13"/>
-      <c r="I23" s="15"/>
-      <c r="J23" s="15"/>
-      <c r="K23" s="15"/>
-      <c r="L23" s="15"/>
-      <c r="M23" s="15"/>
-      <c r="N23" s="17"/>
-      <c r="O23" s="18"/>
-      <c r="P23" s="18"/>
-      <c r="Q23" s="18"/>
-      <c r="R23" s="18"/>
-      <c r="S23" s="18"/>
-      <c r="T23" s="18"/>
-      <c r="U23" s="18"/>
-      <c r="V23" s="18"/>
-      <c r="W23" s="19"/>
-      <c r="X23" s="9"/>
+      <c r="H23" s="11"/>
+      <c r="I23" s="13"/>
+      <c r="J23" s="13"/>
+      <c r="K23" s="13"/>
+      <c r="L23" s="13"/>
+      <c r="M23" s="13"/>
+      <c r="N23" s="15"/>
+      <c r="O23" s="16"/>
+      <c r="P23" s="16"/>
+      <c r="Q23" s="16"/>
+      <c r="R23" s="16"/>
+      <c r="S23" s="16"/>
+      <c r="T23" s="16"/>
+      <c r="U23" s="16"/>
+      <c r="V23" s="16"/>
+      <c r="W23" s="17"/>
+      <c r="X23" s="27"/>
       <c r="Y23" s="1"/>
       <c r="Z23" s="1"/>
       <c r="AA23" s="1"/>
@@ -3414,7 +3257,7 @@
       <c r="CM23" s="1"/>
     </row>
     <row r="24" spans="1:91" x14ac:dyDescent="0.25">
-      <c r="A24" s="27">
+      <c r="A24" s="25">
         <v>23</v>
       </c>
       <c r="B24" s="3"/>
@@ -3423,23 +3266,23 @@
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
       <c r="G24" s="4"/>
-      <c r="H24" s="13"/>
-      <c r="I24" s="15"/>
-      <c r="J24" s="15"/>
-      <c r="K24" s="15"/>
-      <c r="L24" s="15"/>
-      <c r="M24" s="15"/>
-      <c r="N24" s="17"/>
-      <c r="O24" s="18"/>
-      <c r="P24" s="18"/>
-      <c r="Q24" s="18"/>
-      <c r="R24" s="18"/>
-      <c r="S24" s="18"/>
-      <c r="T24" s="18"/>
-      <c r="U24" s="18"/>
-      <c r="V24" s="18"/>
-      <c r="W24" s="19"/>
-      <c r="X24" s="9"/>
+      <c r="H24" s="11"/>
+      <c r="I24" s="13"/>
+      <c r="J24" s="13"/>
+      <c r="K24" s="13"/>
+      <c r="L24" s="13"/>
+      <c r="M24" s="13"/>
+      <c r="N24" s="15"/>
+      <c r="O24" s="16"/>
+      <c r="P24" s="16"/>
+      <c r="Q24" s="16"/>
+      <c r="R24" s="16"/>
+      <c r="S24" s="16"/>
+      <c r="T24" s="16"/>
+      <c r="U24" s="16"/>
+      <c r="V24" s="16"/>
+      <c r="W24" s="17"/>
+      <c r="X24" s="27"/>
       <c r="Y24" s="1"/>
       <c r="Z24" s="1"/>
       <c r="AA24" s="1"/>
@@ -3509,7 +3352,7 @@
       <c r="CM24" s="1"/>
     </row>
     <row r="25" spans="1:91" x14ac:dyDescent="0.25">
-      <c r="A25" s="27">
+      <c r="A25" s="25">
         <v>24</v>
       </c>
       <c r="B25" s="3"/>
@@ -3518,23 +3361,23 @@
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
       <c r="G25" s="4"/>
-      <c r="H25" s="13"/>
-      <c r="I25" s="15"/>
-      <c r="J25" s="15"/>
-      <c r="K25" s="15"/>
-      <c r="L25" s="15"/>
-      <c r="M25" s="15"/>
-      <c r="N25" s="17"/>
-      <c r="O25" s="18"/>
-      <c r="P25" s="18"/>
-      <c r="Q25" s="18"/>
-      <c r="R25" s="18"/>
-      <c r="S25" s="18"/>
-      <c r="T25" s="18"/>
-      <c r="U25" s="18"/>
-      <c r="V25" s="18"/>
-      <c r="W25" s="19"/>
-      <c r="X25" s="9"/>
+      <c r="H25" s="11"/>
+      <c r="I25" s="13"/>
+      <c r="J25" s="13"/>
+      <c r="K25" s="13"/>
+      <c r="L25" s="13"/>
+      <c r="M25" s="13"/>
+      <c r="N25" s="15"/>
+      <c r="O25" s="16"/>
+      <c r="P25" s="16"/>
+      <c r="Q25" s="16"/>
+      <c r="R25" s="16"/>
+      <c r="S25" s="16"/>
+      <c r="T25" s="16"/>
+      <c r="U25" s="16"/>
+      <c r="V25" s="16"/>
+      <c r="W25" s="17"/>
+      <c r="X25" s="27"/>
       <c r="Y25" s="1"/>
       <c r="Z25" s="1"/>
       <c r="AA25" s="1"/>
@@ -3604,7 +3447,7 @@
       <c r="CM25" s="1"/>
     </row>
     <row r="26" spans="1:91" x14ac:dyDescent="0.25">
-      <c r="A26" s="27">
+      <c r="A26" s="25">
         <v>25</v>
       </c>
       <c r="B26" s="3"/>
@@ -3613,23 +3456,23 @@
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
       <c r="G26" s="4"/>
-      <c r="H26" s="13"/>
-      <c r="I26" s="15"/>
-      <c r="J26" s="15"/>
-      <c r="K26" s="15"/>
-      <c r="L26" s="15"/>
-      <c r="M26" s="15"/>
-      <c r="N26" s="17"/>
-      <c r="O26" s="18"/>
-      <c r="P26" s="18"/>
-      <c r="Q26" s="18"/>
-      <c r="R26" s="18"/>
-      <c r="S26" s="18"/>
-      <c r="T26" s="18"/>
-      <c r="U26" s="18"/>
-      <c r="V26" s="18"/>
-      <c r="W26" s="19"/>
-      <c r="X26" s="9"/>
+      <c r="H26" s="11"/>
+      <c r="I26" s="13"/>
+      <c r="J26" s="13"/>
+      <c r="K26" s="13"/>
+      <c r="L26" s="13"/>
+      <c r="M26" s="13"/>
+      <c r="N26" s="15"/>
+      <c r="O26" s="16"/>
+      <c r="P26" s="16"/>
+      <c r="Q26" s="16"/>
+      <c r="R26" s="16"/>
+      <c r="S26" s="16"/>
+      <c r="T26" s="16"/>
+      <c r="U26" s="16"/>
+      <c r="V26" s="16"/>
+      <c r="W26" s="17"/>
+      <c r="X26" s="27"/>
       <c r="Y26" s="1"/>
       <c r="Z26" s="1"/>
       <c r="AA26" s="1"/>
@@ -3699,7 +3542,7 @@
       <c r="CM26" s="1"/>
     </row>
     <row r="27" spans="1:91" x14ac:dyDescent="0.25">
-      <c r="A27" s="27">
+      <c r="A27" s="25">
         <v>26</v>
       </c>
       <c r="B27" s="3"/>
@@ -3708,23 +3551,23 @@
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
       <c r="G27" s="4"/>
-      <c r="H27" s="13"/>
-      <c r="I27" s="15"/>
-      <c r="J27" s="15"/>
-      <c r="K27" s="15"/>
-      <c r="L27" s="15"/>
-      <c r="M27" s="15"/>
-      <c r="N27" s="17"/>
-      <c r="O27" s="18"/>
-      <c r="P27" s="18"/>
-      <c r="Q27" s="18"/>
-      <c r="R27" s="18"/>
-      <c r="S27" s="18"/>
-      <c r="T27" s="18"/>
-      <c r="U27" s="18"/>
-      <c r="V27" s="18"/>
-      <c r="W27" s="19"/>
-      <c r="X27" s="9"/>
+      <c r="H27" s="11"/>
+      <c r="I27" s="13"/>
+      <c r="J27" s="13"/>
+      <c r="K27" s="13"/>
+      <c r="L27" s="13"/>
+      <c r="M27" s="13"/>
+      <c r="N27" s="15"/>
+      <c r="O27" s="16"/>
+      <c r="P27" s="16"/>
+      <c r="Q27" s="16"/>
+      <c r="R27" s="16"/>
+      <c r="S27" s="16"/>
+      <c r="T27" s="16"/>
+      <c r="U27" s="16"/>
+      <c r="V27" s="16"/>
+      <c r="W27" s="17"/>
+      <c r="X27" s="27"/>
       <c r="Y27" s="1"/>
       <c r="Z27" s="1"/>
       <c r="AA27" s="1"/>
@@ -3794,7 +3637,7 @@
       <c r="CM27" s="1"/>
     </row>
     <row r="28" spans="1:91" x14ac:dyDescent="0.25">
-      <c r="A28" s="27">
+      <c r="A28" s="25">
         <v>27</v>
       </c>
       <c r="B28" s="3"/>
@@ -3803,23 +3646,23 @@
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
       <c r="G28" s="4"/>
-      <c r="H28" s="13"/>
-      <c r="I28" s="15"/>
-      <c r="J28" s="15"/>
-      <c r="K28" s="15"/>
-      <c r="L28" s="15"/>
-      <c r="M28" s="15"/>
-      <c r="N28" s="17"/>
-      <c r="O28" s="18"/>
-      <c r="P28" s="18"/>
-      <c r="Q28" s="18"/>
-      <c r="R28" s="18"/>
-      <c r="S28" s="18"/>
-      <c r="T28" s="18"/>
-      <c r="U28" s="18"/>
-      <c r="V28" s="18"/>
-      <c r="W28" s="19"/>
-      <c r="X28" s="9"/>
+      <c r="H28" s="11"/>
+      <c r="I28" s="13"/>
+      <c r="J28" s="13"/>
+      <c r="K28" s="13"/>
+      <c r="L28" s="13"/>
+      <c r="M28" s="13"/>
+      <c r="N28" s="15"/>
+      <c r="O28" s="16"/>
+      <c r="P28" s="16"/>
+      <c r="Q28" s="16"/>
+      <c r="R28" s="16"/>
+      <c r="S28" s="16"/>
+      <c r="T28" s="16"/>
+      <c r="U28" s="16"/>
+      <c r="V28" s="16"/>
+      <c r="W28" s="17"/>
+      <c r="X28" s="27"/>
       <c r="Y28" s="1"/>
       <c r="Z28" s="1"/>
       <c r="AA28" s="1"/>
@@ -3889,7 +3732,7 @@
       <c r="CM28" s="1"/>
     </row>
     <row r="29" spans="1:91" x14ac:dyDescent="0.25">
-      <c r="A29" s="27">
+      <c r="A29" s="25">
         <v>28</v>
       </c>
       <c r="B29" s="3"/>
@@ -3898,23 +3741,23 @@
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
       <c r="G29" s="4"/>
-      <c r="H29" s="13"/>
-      <c r="I29" s="15"/>
-      <c r="J29" s="15"/>
-      <c r="K29" s="15"/>
-      <c r="L29" s="15"/>
-      <c r="M29" s="15"/>
-      <c r="N29" s="17"/>
-      <c r="O29" s="18"/>
-      <c r="P29" s="18"/>
-      <c r="Q29" s="18"/>
-      <c r="R29" s="18"/>
-      <c r="S29" s="18"/>
-      <c r="T29" s="18"/>
-      <c r="U29" s="18"/>
-      <c r="V29" s="18"/>
-      <c r="W29" s="19"/>
-      <c r="X29" s="9"/>
+      <c r="H29" s="11"/>
+      <c r="I29" s="13"/>
+      <c r="J29" s="13"/>
+      <c r="K29" s="13"/>
+      <c r="L29" s="13"/>
+      <c r="M29" s="13"/>
+      <c r="N29" s="15"/>
+      <c r="O29" s="16"/>
+      <c r="P29" s="16"/>
+      <c r="Q29" s="16"/>
+      <c r="R29" s="16"/>
+      <c r="S29" s="16"/>
+      <c r="T29" s="16"/>
+      <c r="U29" s="16"/>
+      <c r="V29" s="16"/>
+      <c r="W29" s="17"/>
+      <c r="X29" s="27"/>
       <c r="Y29" s="1"/>
       <c r="Z29" s="1"/>
       <c r="AA29" s="1"/>
@@ -3984,7 +3827,7 @@
       <c r="CM29" s="1"/>
     </row>
     <row r="30" spans="1:91" x14ac:dyDescent="0.25">
-      <c r="A30" s="27">
+      <c r="A30" s="25">
         <v>29</v>
       </c>
       <c r="B30" s="3"/>
@@ -3993,23 +3836,23 @@
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
       <c r="G30" s="4"/>
-      <c r="H30" s="13"/>
-      <c r="I30" s="15"/>
-      <c r="J30" s="15"/>
-      <c r="K30" s="15"/>
-      <c r="L30" s="15"/>
-      <c r="M30" s="15"/>
-      <c r="N30" s="17"/>
-      <c r="O30" s="18"/>
-      <c r="P30" s="18"/>
-      <c r="Q30" s="18"/>
-      <c r="R30" s="18"/>
-      <c r="S30" s="18"/>
-      <c r="T30" s="18"/>
-      <c r="U30" s="18"/>
-      <c r="V30" s="18"/>
-      <c r="W30" s="19"/>
-      <c r="X30" s="9"/>
+      <c r="H30" s="11"/>
+      <c r="I30" s="13"/>
+      <c r="J30" s="13"/>
+      <c r="K30" s="13"/>
+      <c r="L30" s="13"/>
+      <c r="M30" s="13"/>
+      <c r="N30" s="15"/>
+      <c r="O30" s="16"/>
+      <c r="P30" s="16"/>
+      <c r="Q30" s="16"/>
+      <c r="R30" s="16"/>
+      <c r="S30" s="16"/>
+      <c r="T30" s="16"/>
+      <c r="U30" s="16"/>
+      <c r="V30" s="16"/>
+      <c r="W30" s="17"/>
+      <c r="X30" s="27"/>
       <c r="Y30" s="1"/>
       <c r="Z30" s="1"/>
       <c r="AA30" s="1"/>
@@ -4079,7 +3922,7 @@
       <c r="CM30" s="1"/>
     </row>
     <row r="31" spans="1:91" x14ac:dyDescent="0.25">
-      <c r="A31" s="27">
+      <c r="A31" s="25">
         <v>30</v>
       </c>
       <c r="B31" s="3"/>
@@ -4088,23 +3931,23 @@
       <c r="E31" s="4"/>
       <c r="F31" s="4"/>
       <c r="G31" s="4"/>
-      <c r="H31" s="13"/>
-      <c r="I31" s="15"/>
-      <c r="J31" s="15"/>
-      <c r="K31" s="15"/>
-      <c r="L31" s="15"/>
-      <c r="M31" s="15"/>
-      <c r="N31" s="17"/>
-      <c r="O31" s="18"/>
-      <c r="P31" s="18"/>
-      <c r="Q31" s="18"/>
-      <c r="R31" s="18"/>
-      <c r="S31" s="18"/>
-      <c r="T31" s="18"/>
-      <c r="U31" s="18"/>
-      <c r="V31" s="18"/>
-      <c r="W31" s="19"/>
-      <c r="X31" s="9"/>
+      <c r="H31" s="11"/>
+      <c r="I31" s="13"/>
+      <c r="J31" s="13"/>
+      <c r="K31" s="13"/>
+      <c r="L31" s="13"/>
+      <c r="M31" s="13"/>
+      <c r="N31" s="15"/>
+      <c r="O31" s="16"/>
+      <c r="P31" s="16"/>
+      <c r="Q31" s="16"/>
+      <c r="R31" s="16"/>
+      <c r="S31" s="16"/>
+      <c r="T31" s="16"/>
+      <c r="U31" s="16"/>
+      <c r="V31" s="16"/>
+      <c r="W31" s="17"/>
+      <c r="X31" s="27"/>
       <c r="Y31" s="1"/>
       <c r="Z31" s="1"/>
       <c r="AA31" s="1"/>
@@ -4174,7 +4017,7 @@
       <c r="CM31" s="1"/>
     </row>
     <row r="32" spans="1:91" x14ac:dyDescent="0.25">
-      <c r="A32" s="27">
+      <c r="A32" s="25">
         <v>31</v>
       </c>
       <c r="B32" s="3"/>
@@ -4183,23 +4026,23 @@
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
       <c r="G32" s="4"/>
-      <c r="H32" s="13"/>
-      <c r="I32" s="15"/>
-      <c r="J32" s="15"/>
-      <c r="K32" s="15"/>
-      <c r="L32" s="15"/>
-      <c r="M32" s="15"/>
-      <c r="N32" s="17"/>
-      <c r="O32" s="18"/>
-      <c r="P32" s="18"/>
-      <c r="Q32" s="18"/>
-      <c r="R32" s="18"/>
-      <c r="S32" s="18"/>
-      <c r="T32" s="18"/>
-      <c r="U32" s="18"/>
-      <c r="V32" s="18"/>
-      <c r="W32" s="19"/>
-      <c r="X32" s="9"/>
+      <c r="H32" s="11"/>
+      <c r="I32" s="13"/>
+      <c r="J32" s="13"/>
+      <c r="K32" s="13"/>
+      <c r="L32" s="13"/>
+      <c r="M32" s="13"/>
+      <c r="N32" s="15"/>
+      <c r="O32" s="16"/>
+      <c r="P32" s="16"/>
+      <c r="Q32" s="16"/>
+      <c r="R32" s="16"/>
+      <c r="S32" s="16"/>
+      <c r="T32" s="16"/>
+      <c r="U32" s="16"/>
+      <c r="V32" s="16"/>
+      <c r="W32" s="17"/>
+      <c r="X32" s="27"/>
       <c r="Y32" s="1"/>
       <c r="Z32" s="1"/>
       <c r="AA32" s="1"/>
@@ -4269,7 +4112,7 @@
       <c r="CM32" s="1"/>
     </row>
     <row r="33" spans="1:91" x14ac:dyDescent="0.25">
-      <c r="A33" s="27">
+      <c r="A33" s="25">
         <v>32</v>
       </c>
       <c r="B33" s="3"/>
@@ -4278,23 +4121,23 @@
       <c r="E33" s="4"/>
       <c r="F33" s="4"/>
       <c r="G33" s="4"/>
-      <c r="H33" s="13"/>
-      <c r="I33" s="15"/>
-      <c r="J33" s="15"/>
-      <c r="K33" s="15"/>
-      <c r="L33" s="15"/>
-      <c r="M33" s="15"/>
-      <c r="N33" s="17"/>
-      <c r="O33" s="18"/>
-      <c r="P33" s="18"/>
-      <c r="Q33" s="18"/>
-      <c r="R33" s="18"/>
-      <c r="S33" s="18"/>
-      <c r="T33" s="18"/>
-      <c r="U33" s="18"/>
-      <c r="V33" s="18"/>
-      <c r="W33" s="19"/>
-      <c r="X33" s="9"/>
+      <c r="H33" s="11"/>
+      <c r="I33" s="13"/>
+      <c r="J33" s="13"/>
+      <c r="K33" s="13"/>
+      <c r="L33" s="13"/>
+      <c r="M33" s="13"/>
+      <c r="N33" s="15"/>
+      <c r="O33" s="16"/>
+      <c r="P33" s="16"/>
+      <c r="Q33" s="16"/>
+      <c r="R33" s="16"/>
+      <c r="S33" s="16"/>
+      <c r="T33" s="16"/>
+      <c r="U33" s="16"/>
+      <c r="V33" s="16"/>
+      <c r="W33" s="17"/>
+      <c r="X33" s="27"/>
       <c r="Y33" s="1"/>
       <c r="Z33" s="1"/>
       <c r="AA33" s="1"/>
@@ -4364,7 +4207,7 @@
       <c r="CM33" s="1"/>
     </row>
     <row r="34" spans="1:91" x14ac:dyDescent="0.25">
-      <c r="A34" s="27">
+      <c r="A34" s="25">
         <v>33</v>
       </c>
       <c r="B34" s="3"/>
@@ -4373,23 +4216,23 @@
       <c r="E34" s="4"/>
       <c r="F34" s="4"/>
       <c r="G34" s="4"/>
-      <c r="H34" s="13"/>
-      <c r="I34" s="15"/>
-      <c r="J34" s="15"/>
-      <c r="K34" s="15"/>
-      <c r="L34" s="15"/>
-      <c r="M34" s="15"/>
-      <c r="N34" s="17"/>
-      <c r="O34" s="18"/>
-      <c r="P34" s="18"/>
-      <c r="Q34" s="18"/>
-      <c r="R34" s="18"/>
-      <c r="S34" s="18"/>
-      <c r="T34" s="18"/>
-      <c r="U34" s="18"/>
-      <c r="V34" s="18"/>
-      <c r="W34" s="19"/>
-      <c r="X34" s="9"/>
+      <c r="H34" s="11"/>
+      <c r="I34" s="13"/>
+      <c r="J34" s="13"/>
+      <c r="K34" s="13"/>
+      <c r="L34" s="13"/>
+      <c r="M34" s="13"/>
+      <c r="N34" s="15"/>
+      <c r="O34" s="16"/>
+      <c r="P34" s="16"/>
+      <c r="Q34" s="16"/>
+      <c r="R34" s="16"/>
+      <c r="S34" s="16"/>
+      <c r="T34" s="16"/>
+      <c r="U34" s="16"/>
+      <c r="V34" s="16"/>
+      <c r="W34" s="17"/>
+      <c r="X34" s="27"/>
       <c r="Y34" s="1"/>
       <c r="Z34" s="1"/>
       <c r="AA34" s="1"/>
@@ -4459,7 +4302,7 @@
       <c r="CM34" s="1"/>
     </row>
     <row r="35" spans="1:91" x14ac:dyDescent="0.25">
-      <c r="A35" s="27">
+      <c r="A35" s="25">
         <v>34</v>
       </c>
       <c r="B35" s="3"/>
@@ -4468,23 +4311,23 @@
       <c r="E35" s="4"/>
       <c r="F35" s="4"/>
       <c r="G35" s="4"/>
-      <c r="H35" s="13"/>
-      <c r="I35" s="15"/>
-      <c r="J35" s="15"/>
-      <c r="K35" s="15"/>
-      <c r="L35" s="15"/>
-      <c r="M35" s="15"/>
-      <c r="N35" s="17"/>
-      <c r="O35" s="18"/>
-      <c r="P35" s="18"/>
-      <c r="Q35" s="18"/>
-      <c r="R35" s="18"/>
-      <c r="S35" s="18"/>
-      <c r="T35" s="18"/>
-      <c r="U35" s="18"/>
-      <c r="V35" s="18"/>
-      <c r="W35" s="19"/>
-      <c r="X35" s="9"/>
+      <c r="H35" s="11"/>
+      <c r="I35" s="13"/>
+      <c r="J35" s="13"/>
+      <c r="K35" s="13"/>
+      <c r="L35" s="13"/>
+      <c r="M35" s="13"/>
+      <c r="N35" s="15"/>
+      <c r="O35" s="16"/>
+      <c r="P35" s="16"/>
+      <c r="Q35" s="16"/>
+      <c r="R35" s="16"/>
+      <c r="S35" s="16"/>
+      <c r="T35" s="16"/>
+      <c r="U35" s="16"/>
+      <c r="V35" s="16"/>
+      <c r="W35" s="17"/>
+      <c r="X35" s="27"/>
       <c r="Y35" s="1"/>
       <c r="Z35" s="1"/>
       <c r="AA35" s="1"/>
@@ -4554,7 +4397,7 @@
       <c r="CM35" s="1"/>
     </row>
     <row r="36" spans="1:91" x14ac:dyDescent="0.25">
-      <c r="A36" s="27">
+      <c r="A36" s="25">
         <v>35</v>
       </c>
       <c r="B36" s="3"/>
@@ -4563,23 +4406,23 @@
       <c r="E36" s="4"/>
       <c r="F36" s="4"/>
       <c r="G36" s="4"/>
-      <c r="H36" s="13"/>
-      <c r="I36" s="15"/>
-      <c r="J36" s="15"/>
-      <c r="K36" s="15"/>
-      <c r="L36" s="15"/>
-      <c r="M36" s="15"/>
-      <c r="N36" s="17"/>
-      <c r="O36" s="18"/>
-      <c r="P36" s="18"/>
-      <c r="Q36" s="18"/>
-      <c r="R36" s="18"/>
-      <c r="S36" s="18"/>
-      <c r="T36" s="18"/>
-      <c r="U36" s="18"/>
-      <c r="V36" s="18"/>
-      <c r="W36" s="19"/>
-      <c r="X36" s="9"/>
+      <c r="H36" s="11"/>
+      <c r="I36" s="13"/>
+      <c r="J36" s="13"/>
+      <c r="K36" s="13"/>
+      <c r="L36" s="13"/>
+      <c r="M36" s="13"/>
+      <c r="N36" s="15"/>
+      <c r="O36" s="16"/>
+      <c r="P36" s="16"/>
+      <c r="Q36" s="16"/>
+      <c r="R36" s="16"/>
+      <c r="S36" s="16"/>
+      <c r="T36" s="16"/>
+      <c r="U36" s="16"/>
+      <c r="V36" s="16"/>
+      <c r="W36" s="17"/>
+      <c r="X36" s="27"/>
       <c r="Y36" s="1"/>
       <c r="Z36" s="1"/>
       <c r="AA36" s="1"/>
@@ -4649,7 +4492,7 @@
       <c r="CM36" s="1"/>
     </row>
     <row r="37" spans="1:91" x14ac:dyDescent="0.25">
-      <c r="A37" s="27">
+      <c r="A37" s="25">
         <v>36</v>
       </c>
       <c r="B37" s="3"/>
@@ -4658,23 +4501,23 @@
       <c r="E37" s="4"/>
       <c r="F37" s="4"/>
       <c r="G37" s="4"/>
-      <c r="H37" s="13"/>
-      <c r="I37" s="15"/>
-      <c r="J37" s="15"/>
-      <c r="K37" s="15"/>
-      <c r="L37" s="15"/>
-      <c r="M37" s="15"/>
-      <c r="N37" s="17"/>
-      <c r="O37" s="18"/>
-      <c r="P37" s="18"/>
-      <c r="Q37" s="18"/>
-      <c r="R37" s="18"/>
-      <c r="S37" s="18"/>
-      <c r="T37" s="18"/>
-      <c r="U37" s="18"/>
-      <c r="V37" s="18"/>
-      <c r="W37" s="19"/>
-      <c r="X37" s="9"/>
+      <c r="H37" s="11"/>
+      <c r="I37" s="13"/>
+      <c r="J37" s="13"/>
+      <c r="K37" s="13"/>
+      <c r="L37" s="13"/>
+      <c r="M37" s="13"/>
+      <c r="N37" s="15"/>
+      <c r="O37" s="16"/>
+      <c r="P37" s="16"/>
+      <c r="Q37" s="16"/>
+      <c r="R37" s="16"/>
+      <c r="S37" s="16"/>
+      <c r="T37" s="16"/>
+      <c r="U37" s="16"/>
+      <c r="V37" s="16"/>
+      <c r="W37" s="17"/>
+      <c r="X37" s="27"/>
       <c r="Y37" s="1"/>
       <c r="Z37" s="1"/>
       <c r="AA37" s="1"/>
@@ -4744,7 +4587,7 @@
       <c r="CM37" s="1"/>
     </row>
     <row r="38" spans="1:91" x14ac:dyDescent="0.25">
-      <c r="A38" s="27">
+      <c r="A38" s="25">
         <v>37</v>
       </c>
       <c r="B38" s="3"/>
@@ -4753,23 +4596,23 @@
       <c r="E38" s="4"/>
       <c r="F38" s="4"/>
       <c r="G38" s="4"/>
-      <c r="H38" s="13"/>
-      <c r="I38" s="15"/>
-      <c r="J38" s="15"/>
-      <c r="K38" s="15"/>
-      <c r="L38" s="15"/>
-      <c r="M38" s="15"/>
-      <c r="N38" s="17"/>
-      <c r="O38" s="18"/>
-      <c r="P38" s="18"/>
-      <c r="Q38" s="18"/>
-      <c r="R38" s="18"/>
-      <c r="S38" s="18"/>
-      <c r="T38" s="18"/>
-      <c r="U38" s="18"/>
-      <c r="V38" s="18"/>
-      <c r="W38" s="19"/>
-      <c r="X38" s="9"/>
+      <c r="H38" s="11"/>
+      <c r="I38" s="13"/>
+      <c r="J38" s="13"/>
+      <c r="K38" s="13"/>
+      <c r="L38" s="13"/>
+      <c r="M38" s="13"/>
+      <c r="N38" s="15"/>
+      <c r="O38" s="16"/>
+      <c r="P38" s="16"/>
+      <c r="Q38" s="16"/>
+      <c r="R38" s="16"/>
+      <c r="S38" s="16"/>
+      <c r="T38" s="16"/>
+      <c r="U38" s="16"/>
+      <c r="V38" s="16"/>
+      <c r="W38" s="17"/>
+      <c r="X38" s="27"/>
       <c r="Y38" s="1"/>
       <c r="Z38" s="1"/>
       <c r="AA38" s="1"/>
@@ -4839,7 +4682,7 @@
       <c r="CM38" s="1"/>
     </row>
     <row r="39" spans="1:91" x14ac:dyDescent="0.25">
-      <c r="A39" s="27">
+      <c r="A39" s="25">
         <v>38</v>
       </c>
       <c r="B39" s="3"/>
@@ -4848,23 +4691,23 @@
       <c r="E39" s="4"/>
       <c r="F39" s="4"/>
       <c r="G39" s="4"/>
-      <c r="H39" s="13"/>
-      <c r="I39" s="15"/>
-      <c r="J39" s="15"/>
-      <c r="K39" s="15"/>
-      <c r="L39" s="15"/>
-      <c r="M39" s="15"/>
-      <c r="N39" s="17"/>
-      <c r="O39" s="18"/>
-      <c r="P39" s="18"/>
-      <c r="Q39" s="18"/>
-      <c r="R39" s="18"/>
-      <c r="S39" s="18"/>
-      <c r="T39" s="18"/>
-      <c r="U39" s="18"/>
-      <c r="V39" s="18"/>
-      <c r="W39" s="19"/>
-      <c r="X39" s="9"/>
+      <c r="H39" s="11"/>
+      <c r="I39" s="13"/>
+      <c r="J39" s="13"/>
+      <c r="K39" s="13"/>
+      <c r="L39" s="13"/>
+      <c r="M39" s="13"/>
+      <c r="N39" s="15"/>
+      <c r="O39" s="16"/>
+      <c r="P39" s="16"/>
+      <c r="Q39" s="16"/>
+      <c r="R39" s="16"/>
+      <c r="S39" s="16"/>
+      <c r="T39" s="16"/>
+      <c r="U39" s="16"/>
+      <c r="V39" s="16"/>
+      <c r="W39" s="17"/>
+      <c r="X39" s="27"/>
       <c r="Y39" s="1"/>
       <c r="Z39" s="1"/>
       <c r="AA39" s="1"/>
@@ -4934,7 +4777,7 @@
       <c r="CM39" s="1"/>
     </row>
     <row r="40" spans="1:91" x14ac:dyDescent="0.25">
-      <c r="A40" s="27">
+      <c r="A40" s="25">
         <v>39</v>
       </c>
       <c r="B40" s="3"/>
@@ -4943,23 +4786,23 @@
       <c r="E40" s="4"/>
       <c r="F40" s="4"/>
       <c r="G40" s="4"/>
-      <c r="H40" s="13"/>
-      <c r="I40" s="15"/>
-      <c r="J40" s="15"/>
-      <c r="K40" s="15"/>
-      <c r="L40" s="15"/>
-      <c r="M40" s="15"/>
-      <c r="N40" s="17"/>
-      <c r="O40" s="18"/>
-      <c r="P40" s="18"/>
-      <c r="Q40" s="18"/>
-      <c r="R40" s="18"/>
-      <c r="S40" s="18"/>
-      <c r="T40" s="18"/>
-      <c r="U40" s="18"/>
-      <c r="V40" s="18"/>
-      <c r="W40" s="19"/>
-      <c r="X40" s="9"/>
+      <c r="H40" s="11"/>
+      <c r="I40" s="13"/>
+      <c r="J40" s="13"/>
+      <c r="K40" s="13"/>
+      <c r="L40" s="13"/>
+      <c r="M40" s="13"/>
+      <c r="N40" s="15"/>
+      <c r="O40" s="16"/>
+      <c r="P40" s="16"/>
+      <c r="Q40" s="16"/>
+      <c r="R40" s="16"/>
+      <c r="S40" s="16"/>
+      <c r="T40" s="16"/>
+      <c r="U40" s="16"/>
+      <c r="V40" s="16"/>
+      <c r="W40" s="17"/>
+      <c r="X40" s="27"/>
       <c r="Y40" s="1"/>
       <c r="Z40" s="1"/>
       <c r="AA40" s="1"/>
@@ -5029,7 +4872,7 @@
       <c r="CM40" s="1"/>
     </row>
     <row r="41" spans="1:91" x14ac:dyDescent="0.25">
-      <c r="A41" s="27">
+      <c r="A41" s="25">
         <v>40</v>
       </c>
       <c r="B41" s="3"/>
@@ -5038,23 +4881,23 @@
       <c r="E41" s="4"/>
       <c r="F41" s="4"/>
       <c r="G41" s="4"/>
-      <c r="H41" s="13"/>
-      <c r="I41" s="15"/>
-      <c r="J41" s="15"/>
-      <c r="K41" s="15"/>
-      <c r="L41" s="15"/>
-      <c r="M41" s="15"/>
-      <c r="N41" s="17"/>
-      <c r="O41" s="18"/>
-      <c r="P41" s="18"/>
-      <c r="Q41" s="18"/>
-      <c r="R41" s="18"/>
-      <c r="S41" s="18"/>
-      <c r="T41" s="18"/>
-      <c r="U41" s="18"/>
-      <c r="V41" s="18"/>
-      <c r="W41" s="19"/>
-      <c r="X41" s="9"/>
+      <c r="H41" s="11"/>
+      <c r="I41" s="13"/>
+      <c r="J41" s="13"/>
+      <c r="K41" s="13"/>
+      <c r="L41" s="13"/>
+      <c r="M41" s="13"/>
+      <c r="N41" s="15"/>
+      <c r="O41" s="16"/>
+      <c r="P41" s="16"/>
+      <c r="Q41" s="16"/>
+      <c r="R41" s="16"/>
+      <c r="S41" s="16"/>
+      <c r="T41" s="16"/>
+      <c r="U41" s="16"/>
+      <c r="V41" s="16"/>
+      <c r="W41" s="17"/>
+      <c r="X41" s="27"/>
       <c r="Y41" s="1"/>
       <c r="Z41" s="1"/>
       <c r="AA41" s="1"/>
@@ -5124,7 +4967,7 @@
       <c r="CM41" s="1"/>
     </row>
     <row r="42" spans="1:91" x14ac:dyDescent="0.25">
-      <c r="A42" s="27">
+      <c r="A42" s="25">
         <v>41</v>
       </c>
       <c r="B42" s="3"/>
@@ -5133,23 +4976,23 @@
       <c r="E42" s="4"/>
       <c r="F42" s="4"/>
       <c r="G42" s="4"/>
-      <c r="H42" s="13"/>
-      <c r="I42" s="15"/>
-      <c r="J42" s="15"/>
-      <c r="K42" s="15"/>
-      <c r="L42" s="15"/>
-      <c r="M42" s="15"/>
-      <c r="N42" s="17"/>
-      <c r="O42" s="18"/>
-      <c r="P42" s="18"/>
-      <c r="Q42" s="18"/>
-      <c r="R42" s="18"/>
-      <c r="S42" s="18"/>
-      <c r="T42" s="18"/>
-      <c r="U42" s="18"/>
-      <c r="V42" s="18"/>
-      <c r="W42" s="19"/>
-      <c r="X42" s="9"/>
+      <c r="H42" s="11"/>
+      <c r="I42" s="13"/>
+      <c r="J42" s="13"/>
+      <c r="K42" s="13"/>
+      <c r="L42" s="13"/>
+      <c r="M42" s="13"/>
+      <c r="N42" s="15"/>
+      <c r="O42" s="16"/>
+      <c r="P42" s="16"/>
+      <c r="Q42" s="16"/>
+      <c r="R42" s="16"/>
+      <c r="S42" s="16"/>
+      <c r="T42" s="16"/>
+      <c r="U42" s="16"/>
+      <c r="V42" s="16"/>
+      <c r="W42" s="17"/>
+      <c r="X42" s="27"/>
       <c r="Y42" s="1"/>
       <c r="Z42" s="1"/>
       <c r="AA42" s="1"/>
@@ -5219,7 +5062,7 @@
       <c r="CM42" s="1"/>
     </row>
     <row r="43" spans="1:91" x14ac:dyDescent="0.25">
-      <c r="A43" s="27">
+      <c r="A43" s="25">
         <v>42</v>
       </c>
       <c r="B43" s="3"/>
@@ -5228,23 +5071,23 @@
       <c r="E43" s="4"/>
       <c r="F43" s="4"/>
       <c r="G43" s="4"/>
-      <c r="H43" s="13"/>
-      <c r="I43" s="15"/>
-      <c r="J43" s="15"/>
-      <c r="K43" s="15"/>
-      <c r="L43" s="15"/>
-      <c r="M43" s="15"/>
-      <c r="N43" s="17"/>
-      <c r="O43" s="18"/>
-      <c r="P43" s="18"/>
-      <c r="Q43" s="18"/>
-      <c r="R43" s="18"/>
-      <c r="S43" s="18"/>
-      <c r="T43" s="18"/>
-      <c r="U43" s="18"/>
-      <c r="V43" s="18"/>
-      <c r="W43" s="19"/>
-      <c r="X43" s="9"/>
+      <c r="H43" s="11"/>
+      <c r="I43" s="13"/>
+      <c r="J43" s="13"/>
+      <c r="K43" s="13"/>
+      <c r="L43" s="13"/>
+      <c r="M43" s="13"/>
+      <c r="N43" s="15"/>
+      <c r="O43" s="16"/>
+      <c r="P43" s="16"/>
+      <c r="Q43" s="16"/>
+      <c r="R43" s="16"/>
+      <c r="S43" s="16"/>
+      <c r="T43" s="16"/>
+      <c r="U43" s="16"/>
+      <c r="V43" s="16"/>
+      <c r="W43" s="17"/>
+      <c r="X43" s="27"/>
       <c r="Y43" s="1"/>
       <c r="Z43" s="1"/>
       <c r="AA43" s="1"/>
@@ -5314,7 +5157,7 @@
       <c r="CM43" s="1"/>
     </row>
     <row r="44" spans="1:91" x14ac:dyDescent="0.25">
-      <c r="A44" s="27">
+      <c r="A44" s="25">
         <v>43</v>
       </c>
       <c r="B44" s="3"/>
@@ -5323,23 +5166,23 @@
       <c r="E44" s="4"/>
       <c r="F44" s="4"/>
       <c r="G44" s="4"/>
-      <c r="H44" s="13"/>
-      <c r="I44" s="15"/>
-      <c r="J44" s="15"/>
-      <c r="K44" s="15"/>
-      <c r="L44" s="15"/>
-      <c r="M44" s="15"/>
-      <c r="N44" s="17"/>
-      <c r="O44" s="18"/>
-      <c r="P44" s="18"/>
-      <c r="Q44" s="18"/>
-      <c r="R44" s="18"/>
-      <c r="S44" s="18"/>
-      <c r="T44" s="18"/>
-      <c r="U44" s="18"/>
-      <c r="V44" s="18"/>
-      <c r="W44" s="19"/>
-      <c r="X44" s="9"/>
+      <c r="H44" s="11"/>
+      <c r="I44" s="13"/>
+      <c r="J44" s="13"/>
+      <c r="K44" s="13"/>
+      <c r="L44" s="13"/>
+      <c r="M44" s="13"/>
+      <c r="N44" s="15"/>
+      <c r="O44" s="16"/>
+      <c r="P44" s="16"/>
+      <c r="Q44" s="16"/>
+      <c r="R44" s="16"/>
+      <c r="S44" s="16"/>
+      <c r="T44" s="16"/>
+      <c r="U44" s="16"/>
+      <c r="V44" s="16"/>
+      <c r="W44" s="17"/>
+      <c r="X44" s="27"/>
       <c r="Y44" s="1"/>
       <c r="Z44" s="1"/>
       <c r="AA44" s="1"/>
@@ -5409,7 +5252,7 @@
       <c r="CM44" s="1"/>
     </row>
     <row r="45" spans="1:91" x14ac:dyDescent="0.25">
-      <c r="A45" s="27">
+      <c r="A45" s="25">
         <v>44</v>
       </c>
       <c r="B45" s="3"/>
@@ -5418,23 +5261,23 @@
       <c r="E45" s="4"/>
       <c r="F45" s="4"/>
       <c r="G45" s="4"/>
-      <c r="H45" s="13"/>
-      <c r="I45" s="15"/>
-      <c r="J45" s="15"/>
-      <c r="K45" s="15"/>
-      <c r="L45" s="15"/>
-      <c r="M45" s="15"/>
-      <c r="N45" s="17"/>
-      <c r="O45" s="18"/>
-      <c r="P45" s="18"/>
-      <c r="Q45" s="18"/>
-      <c r="R45" s="18"/>
-      <c r="S45" s="18"/>
-      <c r="T45" s="18"/>
-      <c r="U45" s="18"/>
-      <c r="V45" s="18"/>
-      <c r="W45" s="19"/>
-      <c r="X45" s="9"/>
+      <c r="H45" s="11"/>
+      <c r="I45" s="13"/>
+      <c r="J45" s="13"/>
+      <c r="K45" s="13"/>
+      <c r="L45" s="13"/>
+      <c r="M45" s="13"/>
+      <c r="N45" s="15"/>
+      <c r="O45" s="16"/>
+      <c r="P45" s="16"/>
+      <c r="Q45" s="16"/>
+      <c r="R45" s="16"/>
+      <c r="S45" s="16"/>
+      <c r="T45" s="16"/>
+      <c r="U45" s="16"/>
+      <c r="V45" s="16"/>
+      <c r="W45" s="17"/>
+      <c r="X45" s="27"/>
       <c r="Y45" s="1"/>
       <c r="Z45" s="1"/>
       <c r="AA45" s="1"/>
@@ -5504,7 +5347,7 @@
       <c r="CM45" s="1"/>
     </row>
     <row r="46" spans="1:91" x14ac:dyDescent="0.25">
-      <c r="A46" s="27">
+      <c r="A46" s="25">
         <v>45</v>
       </c>
       <c r="B46" s="3"/>
@@ -5513,23 +5356,23 @@
       <c r="E46" s="4"/>
       <c r="F46" s="4"/>
       <c r="G46" s="4"/>
-      <c r="H46" s="13"/>
-      <c r="I46" s="15"/>
-      <c r="J46" s="15"/>
-      <c r="K46" s="15"/>
-      <c r="L46" s="15"/>
-      <c r="M46" s="15"/>
-      <c r="N46" s="17"/>
-      <c r="O46" s="18"/>
-      <c r="P46" s="18"/>
-      <c r="Q46" s="18"/>
-      <c r="R46" s="18"/>
-      <c r="S46" s="18"/>
-      <c r="T46" s="18"/>
-      <c r="U46" s="18"/>
-      <c r="V46" s="18"/>
-      <c r="W46" s="19"/>
-      <c r="X46" s="9"/>
+      <c r="H46" s="11"/>
+      <c r="I46" s="13"/>
+      <c r="J46" s="13"/>
+      <c r="K46" s="13"/>
+      <c r="L46" s="13"/>
+      <c r="M46" s="13"/>
+      <c r="N46" s="15"/>
+      <c r="O46" s="16"/>
+      <c r="P46" s="16"/>
+      <c r="Q46" s="16"/>
+      <c r="R46" s="16"/>
+      <c r="S46" s="16"/>
+      <c r="T46" s="16"/>
+      <c r="U46" s="16"/>
+      <c r="V46" s="16"/>
+      <c r="W46" s="17"/>
+      <c r="X46" s="27"/>
       <c r="Y46" s="1"/>
       <c r="Z46" s="1"/>
       <c r="AA46" s="1"/>
@@ -5599,7 +5442,7 @@
       <c r="CM46" s="1"/>
     </row>
     <row r="47" spans="1:91" x14ac:dyDescent="0.25">
-      <c r="A47" s="27">
+      <c r="A47" s="25">
         <v>46</v>
       </c>
       <c r="B47" s="3"/>
@@ -5608,23 +5451,23 @@
       <c r="E47" s="4"/>
       <c r="F47" s="4"/>
       <c r="G47" s="4"/>
-      <c r="H47" s="13"/>
-      <c r="I47" s="15"/>
-      <c r="J47" s="15"/>
-      <c r="K47" s="15"/>
-      <c r="L47" s="15"/>
-      <c r="M47" s="15"/>
-      <c r="N47" s="17"/>
-      <c r="O47" s="18"/>
-      <c r="P47" s="18"/>
-      <c r="Q47" s="18"/>
-      <c r="R47" s="18"/>
-      <c r="S47" s="18"/>
-      <c r="T47" s="18"/>
-      <c r="U47" s="18"/>
-      <c r="V47" s="18"/>
-      <c r="W47" s="19"/>
-      <c r="X47" s="9"/>
+      <c r="H47" s="11"/>
+      <c r="I47" s="13"/>
+      <c r="J47" s="13"/>
+      <c r="K47" s="13"/>
+      <c r="L47" s="13"/>
+      <c r="M47" s="13"/>
+      <c r="N47" s="15"/>
+      <c r="O47" s="16"/>
+      <c r="P47" s="16"/>
+      <c r="Q47" s="16"/>
+      <c r="R47" s="16"/>
+      <c r="S47" s="16"/>
+      <c r="T47" s="16"/>
+      <c r="U47" s="16"/>
+      <c r="V47" s="16"/>
+      <c r="W47" s="17"/>
+      <c r="X47" s="27"/>
       <c r="Y47" s="1"/>
       <c r="Z47" s="1"/>
       <c r="AA47" s="1"/>
@@ -5694,7 +5537,7 @@
       <c r="CM47" s="1"/>
     </row>
     <row r="48" spans="1:91" x14ac:dyDescent="0.25">
-      <c r="A48" s="27">
+      <c r="A48" s="25">
         <v>47</v>
       </c>
       <c r="B48" s="3"/>
@@ -5703,23 +5546,23 @@
       <c r="E48" s="4"/>
       <c r="F48" s="4"/>
       <c r="G48" s="4"/>
-      <c r="H48" s="13"/>
-      <c r="I48" s="15"/>
-      <c r="J48" s="15"/>
-      <c r="K48" s="15"/>
-      <c r="L48" s="15"/>
-      <c r="M48" s="15"/>
-      <c r="N48" s="17"/>
-      <c r="O48" s="18"/>
-      <c r="P48" s="18"/>
-      <c r="Q48" s="18"/>
-      <c r="R48" s="18"/>
-      <c r="S48" s="18"/>
-      <c r="T48" s="18"/>
-      <c r="U48" s="18"/>
-      <c r="V48" s="18"/>
-      <c r="W48" s="19"/>
-      <c r="X48" s="9"/>
+      <c r="H48" s="11"/>
+      <c r="I48" s="13"/>
+      <c r="J48" s="13"/>
+      <c r="K48" s="13"/>
+      <c r="L48" s="13"/>
+      <c r="M48" s="13"/>
+      <c r="N48" s="15"/>
+      <c r="O48" s="16"/>
+      <c r="P48" s="16"/>
+      <c r="Q48" s="16"/>
+      <c r="R48" s="16"/>
+      <c r="S48" s="16"/>
+      <c r="T48" s="16"/>
+      <c r="U48" s="16"/>
+      <c r="V48" s="16"/>
+      <c r="W48" s="17"/>
+      <c r="X48" s="27"/>
       <c r="Y48" s="1"/>
       <c r="Z48" s="1"/>
       <c r="AA48" s="1"/>
@@ -5789,7 +5632,7 @@
       <c r="CM48" s="1"/>
     </row>
     <row r="49" spans="1:91" x14ac:dyDescent="0.25">
-      <c r="A49" s="27">
+      <c r="A49" s="25">
         <v>48</v>
       </c>
       <c r="B49" s="3"/>
@@ -5798,23 +5641,23 @@
       <c r="E49" s="4"/>
       <c r="F49" s="4"/>
       <c r="G49" s="4"/>
-      <c r="H49" s="13"/>
-      <c r="I49" s="15"/>
-      <c r="J49" s="15"/>
-      <c r="K49" s="15"/>
-      <c r="L49" s="15"/>
-      <c r="M49" s="15"/>
-      <c r="N49" s="17"/>
-      <c r="O49" s="18"/>
-      <c r="P49" s="18"/>
-      <c r="Q49" s="18"/>
-      <c r="R49" s="18"/>
-      <c r="S49" s="18"/>
-      <c r="T49" s="18"/>
-      <c r="U49" s="18"/>
-      <c r="V49" s="18"/>
-      <c r="W49" s="19"/>
-      <c r="X49" s="9"/>
+      <c r="H49" s="11"/>
+      <c r="I49" s="13"/>
+      <c r="J49" s="13"/>
+      <c r="K49" s="13"/>
+      <c r="L49" s="13"/>
+      <c r="M49" s="13"/>
+      <c r="N49" s="15"/>
+      <c r="O49" s="16"/>
+      <c r="P49" s="16"/>
+      <c r="Q49" s="16"/>
+      <c r="R49" s="16"/>
+      <c r="S49" s="16"/>
+      <c r="T49" s="16"/>
+      <c r="U49" s="16"/>
+      <c r="V49" s="16"/>
+      <c r="W49" s="17"/>
+      <c r="X49" s="27"/>
       <c r="Y49" s="1"/>
       <c r="Z49" s="1"/>
       <c r="AA49" s="1"/>
@@ -5884,7 +5727,7 @@
       <c r="CM49" s="1"/>
     </row>
     <row r="50" spans="1:91" x14ac:dyDescent="0.25">
-      <c r="A50" s="27">
+      <c r="A50" s="25">
         <v>49</v>
       </c>
       <c r="B50" s="3"/>
@@ -5893,23 +5736,23 @@
       <c r="E50" s="4"/>
       <c r="F50" s="4"/>
       <c r="G50" s="4"/>
-      <c r="H50" s="13"/>
-      <c r="I50" s="15"/>
-      <c r="J50" s="15"/>
-      <c r="K50" s="15"/>
-      <c r="L50" s="15"/>
-      <c r="M50" s="15"/>
-      <c r="N50" s="17"/>
-      <c r="O50" s="18"/>
-      <c r="P50" s="18"/>
-      <c r="Q50" s="18"/>
-      <c r="R50" s="18"/>
-      <c r="S50" s="18"/>
-      <c r="T50" s="18"/>
-      <c r="U50" s="18"/>
-      <c r="V50" s="18"/>
-      <c r="W50" s="19"/>
-      <c r="X50" s="9"/>
+      <c r="H50" s="11"/>
+      <c r="I50" s="13"/>
+      <c r="J50" s="13"/>
+      <c r="K50" s="13"/>
+      <c r="L50" s="13"/>
+      <c r="M50" s="13"/>
+      <c r="N50" s="15"/>
+      <c r="O50" s="16"/>
+      <c r="P50" s="16"/>
+      <c r="Q50" s="16"/>
+      <c r="R50" s="16"/>
+      <c r="S50" s="16"/>
+      <c r="T50" s="16"/>
+      <c r="U50" s="16"/>
+      <c r="V50" s="16"/>
+      <c r="W50" s="17"/>
+      <c r="X50" s="27"/>
       <c r="Y50" s="1"/>
       <c r="Z50" s="1"/>
       <c r="AA50" s="1"/>
@@ -5979,7 +5822,7 @@
       <c r="CM50" s="1"/>
     </row>
     <row r="51" spans="1:91" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="28">
+      <c r="A51" s="26">
         <v>50</v>
       </c>
       <c r="B51" s="5"/>
@@ -5988,23 +5831,23 @@
       <c r="E51" s="6"/>
       <c r="F51" s="6"/>
       <c r="G51" s="6"/>
-      <c r="H51" s="14"/>
-      <c r="I51" s="16"/>
-      <c r="J51" s="16"/>
-      <c r="K51" s="16"/>
-      <c r="L51" s="16"/>
-      <c r="M51" s="16"/>
-      <c r="N51" s="20"/>
-      <c r="O51" s="21"/>
-      <c r="P51" s="21"/>
-      <c r="Q51" s="21"/>
-      <c r="R51" s="21"/>
-      <c r="S51" s="21"/>
-      <c r="T51" s="21"/>
-      <c r="U51" s="21"/>
-      <c r="V51" s="21"/>
-      <c r="W51" s="22"/>
-      <c r="X51" s="11"/>
+      <c r="H51" s="12"/>
+      <c r="I51" s="14"/>
+      <c r="J51" s="14"/>
+      <c r="K51" s="14"/>
+      <c r="L51" s="14"/>
+      <c r="M51" s="14"/>
+      <c r="N51" s="18"/>
+      <c r="O51" s="19"/>
+      <c r="P51" s="19"/>
+      <c r="Q51" s="19"/>
+      <c r="R51" s="19"/>
+      <c r="S51" s="19"/>
+      <c r="T51" s="19"/>
+      <c r="U51" s="19"/>
+      <c r="V51" s="19"/>
+      <c r="W51" s="20"/>
+      <c r="X51" s="28"/>
       <c r="Y51" s="1"/>
       <c r="Z51" s="1"/>
       <c r="AA51" s="1"/>
@@ -54102,7 +53945,7 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="7">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Sheet2!$B$2:$B$3</xm:f>
@@ -54131,13 +53974,19 @@
           <x14:formula1>
             <xm:f>Sheet2!$F$2:$F$5</xm:f>
           </x14:formula1>
-          <xm:sqref>G2:G51</xm:sqref>
+          <xm:sqref>G3:G51</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Sheet2!$A$2:$A$11</xm:f>
           </x14:formula1>
           <xm:sqref>B2:B51</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Sheet2!$E$2:$E$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>G2</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -54149,8 +53998,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -54183,16 +54032,16 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s">
         <v>3</v>
       </c>
       <c r="E2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -54203,16 +54052,16 @@
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -54220,25 +54069,19 @@
         <v>2012</v>
       </c>
       <c r="D4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2013</v>
       </c>
-      <c r="E5" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">

</xml_diff>